<commit_message>
corrigido a lógica do fluxograma logico
</commit_message>
<xml_diff>
--- a/1.2-exercicio-locadora/1.2-exercicio-locadora.xlsx
+++ b/1.2-exercicio-locadora/1.2-exercicio-locadora.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pichau\OneDrive\Desktop\exercicios-bd-sprint1\exercicios-sprint-1-bd\1.2-exercicio-locadora\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DB4E96EE-7D58-4D0A-81F0-B21864D60E72}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{905815D8-96AC-418B-816B-A09DAEE621B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{98F95FF3-0561-4162-959F-A318D6216DCE}"/>
   </bookViews>
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="42">
-  <si>
-    <t>Concecionaria</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="32">
   <si>
     <t>IdEmpresa</t>
   </si>
@@ -51,33 +48,12 @@
     <t>IdAluguel</t>
   </si>
   <si>
-    <t>IdModelo</t>
-  </si>
-  <si>
-    <t>NomeModelo</t>
-  </si>
-  <si>
-    <t>AnoFabricacao</t>
-  </si>
-  <si>
     <t>Marca</t>
   </si>
   <si>
-    <t>IdMarca</t>
-  </si>
-  <si>
-    <t>NomeMarca</t>
-  </si>
-  <si>
     <t>Placa</t>
   </si>
   <si>
-    <t>IdPlaca</t>
-  </si>
-  <si>
-    <t>Localizacao</t>
-  </si>
-  <si>
     <t>Aluguel</t>
   </si>
   <si>
@@ -120,21 +96,12 @@
     <t>Palio</t>
   </si>
   <si>
-    <t>Sequencia</t>
-  </si>
-  <si>
     <t>PLA-0000</t>
   </si>
   <si>
     <t>PLA-0001</t>
   </si>
   <si>
-    <t>Mogi Das Cruzes - SP</t>
-  </si>
-  <si>
-    <t>São Paulo - SP</t>
-  </si>
-  <si>
     <t>Bruno</t>
   </si>
   <si>
@@ -151,6 +118,9 @@
   </si>
   <si>
     <t>Visa</t>
+  </si>
+  <si>
+    <t>Locadora</t>
   </si>
 </sst>
 </file>
@@ -169,7 +139,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="23">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -191,78 +161,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -395,7 +293,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -417,6 +315,13 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="6" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -426,6 +331,13 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="6" fontId="0" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -442,9 +354,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -452,110 +361,11 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="19" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="6" fontId="0" fillId="19" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="19" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="19" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="6" fontId="0" fillId="19" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="19" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -870,10 +680,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F040242-6D5D-4006-893A-59230885B1C9}">
-  <dimension ref="A1:U11"/>
+  <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+      <selection activeCell="M32" sqref="M32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -896,319 +706,234 @@
     <col min="23" max="23" width="19.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="3"/>
       <c r="E1" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="12"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="11"/>
-      <c r="G1" s="12"/>
-      <c r="I1" s="22" t="s">
+      <c r="F2" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="J2" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="23"/>
-      <c r="K1" s="23"/>
-      <c r="L1" s="24"/>
-      <c r="N1" s="36" t="s">
-        <v>11</v>
-      </c>
-      <c r="O1" s="37"/>
-      <c r="P1" s="38"/>
-      <c r="R1" s="48" t="s">
-        <v>14</v>
-      </c>
-      <c r="S1" s="49"/>
-      <c r="T1" s="49"/>
-      <c r="U1" s="50"/>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="G2" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="I2" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="J2" s="26" t="s">
-        <v>9</v>
-      </c>
-      <c r="K2" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="L2" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="N2" s="39" t="s">
-        <v>12</v>
-      </c>
-      <c r="O2" s="40" t="s">
-        <v>13</v>
-      </c>
-      <c r="P2" s="41" t="s">
-        <v>8</v>
-      </c>
-      <c r="R2" s="51" t="s">
-        <v>15</v>
-      </c>
-      <c r="S2" s="52" t="s">
-        <v>31</v>
-      </c>
-      <c r="T2" s="52" t="s">
-        <v>16</v>
-      </c>
-      <c r="U2" s="53" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="7">
         <v>1</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E3" s="16">
         <v>5</v>
       </c>
-      <c r="F3" s="17">
+      <c r="F3" s="40" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="40" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" s="40" t="s">
+        <v>23</v>
+      </c>
+      <c r="I3" s="20">
         <v>1</v>
       </c>
-      <c r="G3" s="18">
+      <c r="J3" s="21">
         <v>6</v>
       </c>
-      <c r="I3" s="28">
+    </row>
+    <row r="4" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E4" s="22">
         <v>2</v>
       </c>
-      <c r="J3" s="29" t="s">
+      <c r="F4" s="41" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="41" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4" s="41" t="s">
+        <v>24</v>
+      </c>
+      <c r="I4" s="26">
+        <v>1</v>
+      </c>
+      <c r="J4" s="27">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="12"/>
+      <c r="H8" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="I8" s="29"/>
+      <c r="J8" s="29"/>
+      <c r="K8" s="29"/>
+      <c r="L8" s="29"/>
+      <c r="M8" s="30"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="H9" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="I9" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="J9" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="K9" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="L9" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="M9" s="33" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="16">
+        <v>6</v>
+      </c>
+      <c r="B10" s="17">
+        <v>43393</v>
+      </c>
+      <c r="C10" s="18">
+        <v>12000</v>
+      </c>
+      <c r="D10" s="19">
+        <v>43424</v>
+      </c>
+      <c r="E10" s="20">
+        <v>5</v>
+      </c>
+      <c r="F10" s="21">
+        <v>50</v>
+      </c>
+      <c r="H10" s="34">
+        <v>50</v>
+      </c>
+      <c r="I10" s="35" t="s">
+        <v>25</v>
+      </c>
+      <c r="J10" s="35" t="s">
+        <v>27</v>
+      </c>
+      <c r="K10" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="K3" s="30">
-        <v>2012</v>
-      </c>
-      <c r="L3" s="31">
-        <v>5</v>
-      </c>
-      <c r="N3" s="42">
-        <v>10</v>
-      </c>
-      <c r="O3" s="43" t="s">
+      <c r="L10" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="P3" s="44">
+      <c r="M10" s="36">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="22">
+        <v>3</v>
+      </c>
+      <c r="B11" s="23">
+        <v>40240</v>
+      </c>
+      <c r="C11" s="24">
+        <v>6000</v>
+      </c>
+      <c r="D11" s="25">
+        <v>40271</v>
+      </c>
+      <c r="E11" s="26">
         <v>2</v>
       </c>
-      <c r="R3" s="54">
-        <v>20</v>
-      </c>
-      <c r="S3" s="55" t="s">
-        <v>32</v>
-      </c>
-      <c r="T3" s="55" t="s">
-        <v>34</v>
-      </c>
-      <c r="U3" s="56">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E4" s="19">
-        <v>2</v>
-      </c>
-      <c r="F4" s="20">
-        <v>1</v>
-      </c>
-      <c r="G4" s="21">
-        <v>3</v>
-      </c>
-      <c r="I4" s="32">
-        <v>3</v>
-      </c>
-      <c r="J4" s="33" t="s">
+      <c r="F11" s="27">
+        <v>55</v>
+      </c>
+      <c r="H11" s="37">
+        <v>55</v>
+      </c>
+      <c r="I11" s="38" t="s">
+        <v>26</v>
+      </c>
+      <c r="J11" s="38" t="s">
+        <v>27</v>
+      </c>
+      <c r="K11" s="38" t="s">
+        <v>28</v>
+      </c>
+      <c r="L11" s="38" t="s">
         <v>30</v>
       </c>
-      <c r="K4" s="34">
-        <v>1996</v>
-      </c>
-      <c r="L4" s="35">
-        <v>2</v>
-      </c>
-      <c r="N4" s="45">
-        <v>10</v>
-      </c>
-      <c r="O4" s="46" t="s">
-        <v>29</v>
-      </c>
-      <c r="P4" s="47">
-        <v>3</v>
-      </c>
-      <c r="R4" s="57">
-        <v>25</v>
-      </c>
-      <c r="S4" s="58" t="s">
-        <v>33</v>
-      </c>
-      <c r="T4" s="58" t="s">
-        <v>35</v>
-      </c>
-      <c r="U4" s="59">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A8" s="60" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" s="61"/>
-      <c r="C8" s="61"/>
-      <c r="D8" s="61"/>
-      <c r="E8" s="61"/>
-      <c r="F8" s="62"/>
-      <c r="H8" s="78" t="s">
-        <v>22</v>
-      </c>
-      <c r="I8" s="79"/>
-      <c r="J8" s="79"/>
-      <c r="K8" s="79"/>
-      <c r="L8" s="79"/>
-      <c r="M8" s="80"/>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A9" s="63" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="64" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="64" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9" s="64" t="s">
-        <v>20</v>
-      </c>
-      <c r="E9" s="64" t="s">
-        <v>5</v>
-      </c>
-      <c r="F9" s="65" t="s">
-        <v>21</v>
-      </c>
-      <c r="H9" s="81" t="s">
-        <v>21</v>
-      </c>
-      <c r="I9" s="82" t="s">
-        <v>23</v>
-      </c>
-      <c r="J9" s="82" t="s">
-        <v>24</v>
-      </c>
-      <c r="K9" s="82" t="s">
-        <v>25</v>
-      </c>
-      <c r="L9" s="82" t="s">
-        <v>26</v>
-      </c>
-      <c r="M9" s="83" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A10" s="66">
-        <v>6</v>
-      </c>
-      <c r="B10" s="67">
-        <v>43393</v>
-      </c>
-      <c r="C10" s="68">
-        <v>12000</v>
-      </c>
-      <c r="D10" s="69">
-        <v>43424</v>
-      </c>
-      <c r="E10" s="70">
-        <v>5</v>
-      </c>
-      <c r="F10" s="71">
-        <v>50</v>
-      </c>
-      <c r="H10" s="84">
-        <v>50</v>
-      </c>
-      <c r="I10" s="85" t="s">
-        <v>36</v>
-      </c>
-      <c r="J10" s="85" t="s">
-        <v>38</v>
-      </c>
-      <c r="K10" s="85" t="s">
-        <v>39</v>
-      </c>
-      <c r="L10" s="85" t="s">
-        <v>40</v>
-      </c>
-      <c r="M10" s="86">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="72">
-        <v>3</v>
-      </c>
-      <c r="B11" s="73">
-        <v>40240</v>
-      </c>
-      <c r="C11" s="74">
-        <v>6000</v>
-      </c>
-      <c r="D11" s="75">
-        <v>40271</v>
-      </c>
-      <c r="E11" s="76">
-        <v>2</v>
-      </c>
-      <c r="F11" s="77">
-        <v>55</v>
-      </c>
-      <c r="H11" s="87">
-        <v>55</v>
-      </c>
-      <c r="I11" s="88" t="s">
-        <v>37</v>
-      </c>
-      <c r="J11" s="88" t="s">
-        <v>38</v>
-      </c>
-      <c r="K11" s="88" t="s">
-        <v>39</v>
-      </c>
-      <c r="L11" s="88" t="s">
-        <v>41</v>
-      </c>
-      <c r="M11" s="89">
+      <c r="M11" s="39">
         <v>3</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
adicionado a ddl 1.2
</commit_message>
<xml_diff>
--- a/1.2-exercicio-locadora/1.2-exercicio-locadora.xlsx
+++ b/1.2-exercicio-locadora/1.2-exercicio-locadora.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pichau\OneDrive\Desktop\exercicios-bd-sprint1\exercicios-sprint-1-bd\1.2-exercicio-locadora\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{905815D8-96AC-418B-816B-A09DAEE621B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5D9032E-3755-4362-A40B-CDE35C890493}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{98F95FF3-0561-4162-959F-A318D6216DCE}"/>
+    <workbookView xWindow="1410" yWindow="3060" windowWidth="21600" windowHeight="11385" xr2:uid="{98F95FF3-0561-4162-959F-A318D6216DCE}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="40">
   <si>
     <t>IdEmpresa</t>
   </si>
@@ -121,6 +121,30 @@
   </si>
   <si>
     <t>Locadora</t>
+  </si>
+  <si>
+    <t>Cor</t>
+  </si>
+  <si>
+    <t>Preto</t>
+  </si>
+  <si>
+    <t>Branco</t>
+  </si>
+  <si>
+    <t>IdModelo</t>
+  </si>
+  <si>
+    <t>NomeModelo</t>
+  </si>
+  <si>
+    <t>AnoFabricacao</t>
+  </si>
+  <si>
+    <t>IdMarca</t>
+  </si>
+  <si>
+    <t>NomeMarca</t>
   </si>
 </sst>
 </file>
@@ -139,7 +163,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -197,6 +221,42 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -293,7 +353,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -366,6 +426,52 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -680,10 +786,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F040242-6D5D-4006-893A-59230885B1C9}">
-  <dimension ref="A1:M11"/>
+  <dimension ref="A1:S11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M32" sqref="M32"/>
+      <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -706,7 +812,7 @@
     <col min="23" max="23" width="19.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>31</v>
       </c>
@@ -718,10 +824,21 @@
       <c r="F1" s="11"/>
       <c r="G1" s="11"/>
       <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="K1" s="43" t="s">
+        <v>5</v>
+      </c>
+      <c r="L1" s="44"/>
+      <c r="M1" s="44"/>
+      <c r="N1" s="44"/>
+      <c r="O1" s="45"/>
+      <c r="Q1" s="57" t="s">
+        <v>7</v>
+      </c>
+      <c r="R1" s="58"/>
+      <c r="S1" s="59"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -735,22 +852,43 @@
         <v>4</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="G2" s="14" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H2" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="I2" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="J2" s="15" t="s">
+      <c r="I2" s="15" t="s">
         <v>6</v>
       </c>
+      <c r="K2" s="46" t="s">
+        <v>35</v>
+      </c>
+      <c r="L2" s="42" t="s">
+        <v>36</v>
+      </c>
+      <c r="M2" s="42" t="s">
+        <v>37</v>
+      </c>
+      <c r="N2" s="42" t="s">
+        <v>38</v>
+      </c>
+      <c r="O2" s="47" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q2" s="60" t="s">
+        <v>38</v>
+      </c>
+      <c r="R2" s="56" t="s">
+        <v>39</v>
+      </c>
+      <c r="S2" s="61" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="3" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="7">
         <v>1</v>
       </c>
@@ -764,43 +902,85 @@
         <v>5</v>
       </c>
       <c r="F3" s="40" t="s">
+        <v>33</v>
+      </c>
+      <c r="G3" s="40" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" s="20">
+        <v>1</v>
+      </c>
+      <c r="I3" s="21">
+        <v>6</v>
+      </c>
+      <c r="K3" s="48">
+        <v>10</v>
+      </c>
+      <c r="L3" s="49" t="s">
         <v>20</v>
       </c>
-      <c r="G3" s="40" t="s">
+      <c r="M3" s="50">
+        <v>2012</v>
+      </c>
+      <c r="N3" s="50">
+        <v>50</v>
+      </c>
+      <c r="O3" s="51">
+        <v>5</v>
+      </c>
+      <c r="Q3" s="62">
+        <v>50</v>
+      </c>
+      <c r="R3" s="63" t="s">
         <v>21</v>
       </c>
-      <c r="H3" s="40" t="s">
-        <v>23</v>
-      </c>
-      <c r="I3" s="20">
-        <v>1</v>
-      </c>
-      <c r="J3" s="21">
-        <v>6</v>
+      <c r="S3" s="64">
+        <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E4" s="22">
         <v>2</v>
       </c>
       <c r="F4" s="41" t="s">
+        <v>34</v>
+      </c>
+      <c r="G4" s="41" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" s="26">
+        <v>1</v>
+      </c>
+      <c r="I4" s="27">
+        <v>3</v>
+      </c>
+      <c r="K4" s="52">
+        <v>11</v>
+      </c>
+      <c r="L4" s="53" t="s">
         <v>22</v>
       </c>
-      <c r="G4" s="41" t="s">
+      <c r="M4" s="54">
+        <v>1996</v>
+      </c>
+      <c r="N4" s="54">
+        <v>50</v>
+      </c>
+      <c r="O4" s="55">
+        <v>2</v>
+      </c>
+      <c r="Q4" s="65">
+        <v>50</v>
+      </c>
+      <c r="R4" s="66" t="s">
         <v>21</v>
       </c>
-      <c r="H4" s="41" t="s">
-        <v>24</v>
-      </c>
-      <c r="I4" s="26">
-        <v>1</v>
-      </c>
-      <c r="J4" s="27">
-        <v>3</v>
+      <c r="S4" s="67">
+        <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
         <v>9</v>
       </c>
@@ -818,7 +998,7 @@
       <c r="L8" s="29"/>
       <c r="M8" s="30"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>6</v>
       </c>
@@ -856,7 +1036,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="16">
         <v>6</v>
       </c>
@@ -894,7 +1074,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="22">
         <v>3</v>
       </c>

</xml_diff>